<commit_message>
Add Stage 3 (B1-B2) evidence
</commit_message>
<xml_diff>
--- a/kanakattack/evidence.xlsx
+++ b/kanakattack/evidence.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UMUT\Desktop\coins\gon testnet\kanakattack\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UMUT\Desktop\coins\gon testnet\0K_kanakattack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA155BFA-6894-46E6-AB50-96C90D06F608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C47E63F7-7A0D-47C8-9C2C-458EA2D00CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="860" firstSheet="1" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="44">
   <si>
     <t>TxHash</t>
   </si>
@@ -164,6 +164,18 @@
   </si>
   <si>
     <t>F65A718639486436E208EBE1AEC7AD1BF2531E18566D75E8903F97FD9CD7D94F</t>
+  </si>
+  <si>
+    <t>2EAB50CBBC1B035073C1B33E9C34B048742633EA12287CCF9E8C75AECA263A9C</t>
+  </si>
+  <si>
+    <t>75BD1A9C756EA7AA850073DB4786F953BF355D76549D508AA0B5CFBD1B6D8417</t>
+  </si>
+  <si>
+    <t>B05C79D763058DAF9BD11171E27FA968DC956355E97A05B98618B02BA77BB81E</t>
+  </si>
+  <si>
+    <t>3A565BEB74FC8FA693CA3C245E355A01927E46A0A6D764BD6F26559C97704DAE</t>
   </si>
 </sst>
 </file>
@@ -560,8 +572,8 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1203,7 +1215,9 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1217,12 +1231,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1237,7 +1251,9 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1251,12 +1267,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Stage 2 (A7-A20) evidence
</commit_message>
<xml_diff>
--- a/kanakattack/evidence.xlsx
+++ b/kanakattack/evidence.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UMUT\Desktop\coins\gon testnet\0K_kanakattack\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UMUT\Desktop\coins\gon testnet\_0K_kanakattack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C47E63F7-7A0D-47C8-9C2C-458EA2D00CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D01567E-6CE6-463D-9E63-A9BB34A0B9D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="860" firstSheet="1" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="860" firstSheet="1" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="90">
   <si>
     <t>TxHash</t>
   </si>
@@ -58,27 +58,12 @@
     <t>ChainID</t>
   </si>
   <si>
-    <t>tx hash on that chain</t>
-  </si>
-  <si>
-    <t>chain id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain	chain id</t>
-  </si>
-  <si>
     <t>ClassID</t>
   </si>
   <si>
     <t>NFTID</t>
   </si>
   <si>
-    <t>ibc class on chain</t>
-  </si>
-  <si>
-    <t>nft id</t>
-  </si>
-  <si>
     <t>TeamName</t>
   </si>
   <si>
@@ -176,13 +161,166 @@
   </si>
   <si>
     <t>3A565BEB74FC8FA693CA3C245E355A01927E46A0A6D764BD6F26559C97704DAE</t>
+  </si>
+  <si>
+    <t>ibc/C6E3DC8FA1CE3A5FDBA795E7409D749704C01EE52BCD63E8AC72A0CA67F57071</t>
+  </si>
+  <si>
+    <t>kattckA7</t>
+  </si>
+  <si>
+    <t>ibc/9CF0D6557A1CC7E5AD475CB77E789FCE403B58A124C3BC097D80B722F49CE52D</t>
+  </si>
+  <si>
+    <t>kattckA8</t>
+  </si>
+  <si>
+    <t>ibc/0AD8655220944A962164A80D3CE55F019AE4E53C02B7FA090748357EA89B5433</t>
+  </si>
+  <si>
+    <t>kattckA9</t>
+  </si>
+  <si>
+    <t>ibc/C6A92564F63322AD07124274415F62C70CE6B01AF3E6FB1D15180E35AFC04ED6</t>
+  </si>
+  <si>
+    <t>kattckA10</t>
+  </si>
+  <si>
+    <t>ibc/A40AEEFB7410A55B8A8D61E0607726630C431DE90C5CE631C92FB17C8F8569C7</t>
+  </si>
+  <si>
+    <t>kattckA11</t>
+  </si>
+  <si>
+    <t>ibc/326C9E54BCE4998D95C2D3F7285BDA883DF5A4AF4419CDF403F36D2457030854</t>
+  </si>
+  <si>
+    <t>kattckA12</t>
+  </si>
+  <si>
+    <t>D388E924787F90AAD0A2CF31EFF9CAABCBD135B412FD0E0F3FCE55CFD311744E</t>
+  </si>
+  <si>
+    <t>308B93CC012912C75671666C1FD038BD3C80FDEE01017C4535B08F18BE3DEDB0</t>
+  </si>
+  <si>
+    <t>FCE4A95F72027C91ACDD83EF97B1261DAE3A8F8A0E774953F86915B325C12B48</t>
+  </si>
+  <si>
+    <t>939BCD6710B2C72BFC5361D9E35CBD027D6461793199D6F566A55AAAD4269E93</t>
+  </si>
+  <si>
+    <t>gon-irishub-1</t>
+  </si>
+  <si>
+    <t>uptick_7000-2</t>
+  </si>
+  <si>
+    <t>07C50973212095F94FF7004EB63FD69A9686CAC5C2A359F20715A349947BE3F8</t>
+  </si>
+  <si>
+    <t>9A6FBAE651DDF947D91B3B2C33C93B96410B6891EEC832152780A695F541A857</t>
+  </si>
+  <si>
+    <t>C3C4300D94927B4549CD24F9DA2D10036DD1A05D286EE659E925D61C8D4977B9</t>
+  </si>
+  <si>
+    <t>F776047D31E640AFC70D2873DAF5B0882A90ADC88D4D12A8CD54F914F3583C6D</t>
+  </si>
+  <si>
+    <t>8BE657E168635F66DA509E277716536CDAE850ABCB1D77E4E31DF01AFE1B96E4</t>
+  </si>
+  <si>
+    <t>3173D9E660DADDB0BFAAEF64C503B1198C88DE0CC2F0F27D098E3EB1302CC6A0</t>
+  </si>
+  <si>
+    <t>ACE20B6EF2B188BB86132EA2F7E22813D27D09E33E9B82CFD22924E98007D3CE</t>
+  </si>
+  <si>
+    <t>474FB64078188869AC624F1EA05F431D0A673619EE38DA9A086633ACE53E76A8</t>
+  </si>
+  <si>
+    <t>uni-6</t>
+  </si>
+  <si>
+    <t>F0C5BE3FB2C289F128710330612EC66334BE794B4C5CBF89193E0F72A442DF26</t>
+  </si>
+  <si>
+    <t>4EB2B26E8AC305825D11A2E53B3A69D3B01748F6442D4EE8371C62252FC7D1CD</t>
+  </si>
+  <si>
+    <t>1CA634C54E4E43B0086817E137780B824CE26D289BD2A2315BAEBEA32A1550D6</t>
+  </si>
+  <si>
+    <t>7066FA3DAFB0087E6D677BF0BF3200C82C237B1919D745E3DB226352E0872FB9</t>
+  </si>
+  <si>
+    <t>5783F2887E5BC464ACA76E577EA5756EE02007BA74E9E387E6B203C135086BD3</t>
+  </si>
+  <si>
+    <t>F0148B29244EED4C8E05983911FBF404D615C84989B7AE42F1FE00A61BCBA630</t>
+  </si>
+  <si>
+    <t>7286C64C665452A4046F0630A48047025732BF25989A1C5AA8D7E1406140B538</t>
+  </si>
+  <si>
+    <t>56A69A720D7862A70F2435D8398EE7A5E2D841867482D62844EEAD8405FF4911</t>
+  </si>
+  <si>
+    <t>6CB1CA870F485519B516D977BF40ECE597C387821456EEF7AF0F3AFDC134FCA6</t>
+  </si>
+  <si>
+    <t>2A1E1516C0F3F0B653E318587C3B42B04B38F988A278BF6EAD21F6433D744275</t>
+  </si>
+  <si>
+    <t>1B5CAA65492EE68DC0FC9861DA60CE2527FF9637E224BA2CF858AB3D3225FE4C</t>
+  </si>
+  <si>
+    <t>F951F523DAD735884F7E5AA1ED4F007D705583A971FE0A0E5350B4A219002EB6</t>
+  </si>
+  <si>
+    <t>19C92B2D2424C3FF2C53B62B5901128A3799581818F5D6E1A18D95ECBE3A7B77</t>
+  </si>
+  <si>
+    <t>A60F88F274FA354EEBD53F85AB2E703BBC942A88A1D5FEFE3059CDC1D890F191</t>
+  </si>
+  <si>
+    <t>710589A5595056015A5C74BDED270406AF2C49689873DBF04C7A99866C1C85E2</t>
+  </si>
+  <si>
+    <t>EE8B85B155476EEE23F70DD889831F00AA366F65AEAEE6F85E163588AF41E4AA</t>
+  </si>
+  <si>
+    <t>D1112BAFECC2759EEF11DD4C233413391D4E45DA07D0AE853B84EF2082ADC869</t>
+  </si>
+  <si>
+    <t>EFBEB8992BF9737A8521CB78684F912EAB061CE37174A101A18B2BF1BFF041FE</t>
+  </si>
+  <si>
+    <t>13F863774E66AEE8F843D99CF54A8656F195E345F135A763B11E9176C1119E4F</t>
+  </si>
+  <si>
+    <t>14E29341578471E1485C1C6ABCEBDFBD45E8C156F789EB35B39C96005CFC144E</t>
+  </si>
+  <si>
+    <t>88AC659D1A3EFFEE9EAA8BA546C1D173EA9C2E11C01D7202E25F3E314B155264</t>
+  </si>
+  <si>
+    <t>B58982D239E6EBEBAFE7F7A1B41805F478B65082067164DDBB306358B20178FB</t>
+  </si>
+  <si>
+    <t>0D007EB6752B6422F7A21548564BA2062668B98D7C368EA0DEDB3BECCF5D660A</t>
+  </si>
+  <si>
+    <t>8DA1080796CBFF157F151227CBC94F227F26626157DC6AE29E1E78D54FDEEF72</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,6 +333,27 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="162"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="162"/>
     </font>
   </fonts>
   <fills count="4">
@@ -246,10 +405,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -265,9 +425,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{690DF072-807E-453B-AC78-1EC6C6EBD67F}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -590,51 +755,51 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="H2" s="4"/>
     </row>
@@ -650,7 +815,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -660,33 +827,558 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -696,33 +1388,75 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+      <c r="A2" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -732,78 +1466,6 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -811,397 +1473,52 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
+      <c r="A2" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+      <c r="A3" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+      <c r="A4" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>56</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1231,12 +1548,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1251,7 +1568,7 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -1267,12 +1584,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1370,32 +1687,32 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1426,10 +1743,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1437,16 +1754,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1477,10 +1794,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1488,16 +1805,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1528,10 +1845,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1539,16 +1856,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1580,10 +1897,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1591,16 +1908,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1615,7 +1932,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1625,18 +1944,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
+      <c r="A2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1651,7 +1970,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1661,18 +1982,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
+      <c r="A2" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>